<commit_message>
tratando de corregir el excel
</commit_message>
<xml_diff>
--- a/public/PROYECTO_FINIQUITO (1).xlsx
+++ b/public/PROYECTO_FINIQUITO (1).xlsx
@@ -1907,8 +1907,8 @@
   </sheetPr>
   <dimension ref="A1:AO120"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AY16" activeCellId="0" sqref="AY16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AK39" activeCellId="0" sqref="AK39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>